<commit_message>
trying to add animation
not finished, roar youll either need to delete it or try to get it to work somehow..
</commit_message>
<xml_diff>
--- a/ProjectDiary_base.xlsx
+++ b/ProjectDiary_base.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MH\Desktop\uni\02_Vienna\Web Mapping\project\github\CO2SpatialFootprint\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MH\Desktop\uni\02_Vienna\Web Mapping\project\offline\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="29">
   <si>
     <t>Christian</t>
   </si>
@@ -96,13 +96,16 @@
     <t>Prettiing up: responsive design,hints and coloring</t>
   </si>
   <si>
-    <t>Circle drawing and others</t>
-  </si>
-  <si>
     <t xml:space="preserve">26.6. </t>
   </si>
   <si>
     <t>online meeting and disc.</t>
+  </si>
+  <si>
+    <t>Circle drawing and finalization</t>
+  </si>
+  <si>
+    <t>Testing and improving</t>
   </si>
 </sst>
 </file>
@@ -282,14 +285,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="16" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -607,7 +610,7 @@
   <dimension ref="A1:Z1000"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L8" sqref="L8"/>
+      <selection activeCell="H6" sqref="H6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15" customHeight="1"/>
@@ -647,14 +650,14 @@
       </c>
       <c r="H1" s="2">
         <f>SUM(H3:H99)+SUM(K3:K99)</f>
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="I1" s="3"/>
-      <c r="J1" s="13" t="s">
+      <c r="J1" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="K1" s="14"/>
-      <c r="L1" s="15"/>
+      <c r="K1" s="15"/>
+      <c r="L1" s="16"/>
       <c r="M1" s="4"/>
       <c r="N1" s="4"/>
       <c r="O1" s="4"/>
@@ -879,23 +882,23 @@
       <c r="D6" s="8"/>
       <c r="E6" s="4"/>
       <c r="F6" s="9"/>
-      <c r="G6" s="16">
-        <v>42912</v>
+      <c r="G6" s="13">
+        <v>42900</v>
       </c>
       <c r="H6" s="4">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="I6" s="9" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="J6" s="8" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="K6" s="4">
         <v>2</v>
       </c>
       <c r="L6" s="9" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="M6" s="4"/>
       <c r="N6" s="4"/>
@@ -919,9 +922,15 @@
       <c r="D7" s="8"/>
       <c r="E7" s="4"/>
       <c r="F7" s="9"/>
-      <c r="G7" s="8"/>
-      <c r="H7" s="4"/>
-      <c r="I7" s="9"/>
+      <c r="G7" s="13">
+        <v>42912</v>
+      </c>
+      <c r="H7" s="4">
+        <v>6</v>
+      </c>
+      <c r="I7" s="9" t="s">
+        <v>27</v>
+      </c>
       <c r="J7" s="8"/>
       <c r="K7" s="4"/>
       <c r="L7" s="9"/>

</xml_diff>